<commit_message>
planning changed and costs added
</commit_message>
<xml_diff>
--- a/Aankopen.xlsx
+++ b/Aankopen.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -44,19 +44,19 @@
     <t>link</t>
   </si>
   <si>
-    <t>https://www.adafruit.com/product/1317</t>
-  </si>
-  <si>
-    <t>$5,95</t>
-  </si>
-  <si>
-    <t>LIPO battery</t>
-  </si>
-  <si>
-    <t>charger</t>
-  </si>
-  <si>
-    <t>https://www.adafruit.com/product/1304</t>
+    <t xml:space="preserve">Micro USB OTG </t>
+  </si>
+  <si>
+    <t>https://nl.aliexpress.com/item/1pc-Micro-USB-Type-B-Male-To-Micro-B-Male-5-Pin-Converter-OTG-Adapter-Lead/32808154910.html?spm=a2g0z.search0104.3.221.23ff22089TknZw&amp;ws_ab_test=searchweb0_0,searchweb201602_1_10152_10151_10065_10344_10068_10342_10343_10340_10341_10084_10083_10618_10630_10304_10307_10302_5711211_10313_10059_5722311_10534_100031_10103_10627_10626_10624_10623_10622_10621_10620_5711311_10142,searchweb201603_25,ppcSwitch_4&amp;algo_expid=24fc4199-da5a-4461-8ea1-e398eb22a66b-29&amp;algo_pvid=24fc4199-da5a-4461-8ea1-e398eb22a66b&amp;priceBeautifyAB=0</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>LiPo Batteries + Charger</t>
+  </si>
+  <si>
+    <t>https://nl.aliexpress.com/item/5pcs-Lipo-Battery-3-7V-150mAh-USB-Lipo-Charger-Set-For-JJRC-H20-Mini-RC-Hexacopter/32791721090.html?spm=a2g0s.13010208.99999999.262.0rynF9</t>
   </si>
 </sst>
 </file>
@@ -64,9 +64,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="&quot;€&quot;\ #,##0.00_);[Red]\(&quot;€&quot;\ #,##0.00\)"/>
+    <numFmt numFmtId="164" formatCode="&quot;€&quot;\ #,##0.00"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -78,6 +78,14 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -104,10 +112,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -423,75 +434,104 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67E89092-BD48-AA4E-B39D-652DD530358D}">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="17.33203125" customWidth="1"/>
+    <col min="2" max="2" width="22.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="L1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="M1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="L2" s="2">
-        <v>120.24</v>
-      </c>
-      <c r="M2">
+      <c r="C2" s="4">
+        <v>116.71</v>
+      </c>
+      <c r="D2" s="3">
         <v>1</v>
       </c>
+      <c r="E2" s="4">
+        <f>C2*D2</f>
+        <v>116.71</v>
+      </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
         <v>6</v>
       </c>
-      <c r="L3" t="s">
+      <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="M3">
-        <v>3</v>
+      <c r="C3" s="4">
+        <v>1.32</v>
+      </c>
+      <c r="D3" s="3">
+        <v>2</v>
+      </c>
+      <c r="E3" s="4">
+        <f t="shared" ref="E3:E4" si="0">C3*D3</f>
+        <v>2.64</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="C4" t="s">
+      <c r="B4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L4" t="s">
-        <v>7</v>
-      </c>
-      <c r="M4">
-        <v>2</v>
+      <c r="C4" s="4">
+        <v>12.47</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1</v>
+      </c>
+      <c r="E4" s="4">
+        <f t="shared" si="0"/>
+        <v>12.47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="5">
+        <f>SUM(E2:E4)</f>
+        <v>131.82</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="https://www.amazon.fr/gp/product/B00FS7SV1U/ref=ox_sc_act_title_1?smid=A1X6FK5RDHNB96&amp;psc=1" xr:uid="{9D829933-FC20-F240-BCB1-D0637A3A892D}"/>
+    <hyperlink ref="B2" r:id="rId1" display="https://www.amazon.fr/gp/product/B00FS7SV1U/ref=ox_sc_act_title_1?smid=A1X6FK5RDHNB96&amp;psc=1" xr:uid="{9D829933-FC20-F240-BCB1-D0637A3A892D}"/>
+    <hyperlink ref="B4" r:id="rId2" xr:uid="{969AD172-4D40-4D95-8A3B-D0CB782DA9E8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>